<commit_message>
fix formatting in advanced excel sample
</commit_message>
<xml_diff>
--- a/src/TaxCalculator.Specs/TaxCalculation-ExcelMagic.feature.xlsx
+++ b/src/TaxCalculator.Specs/TaxCalculation-ExcelMagic.feature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="727"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="727"/>
   </bookViews>
   <sheets>
     <sheet name="Coloring" sheetId="11" r:id="rId1"/>
@@ -14,8 +14,8 @@
     <sheet name="_Taxes2013" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable41" hidden="1">[0]!Table4</definedName>
-    <definedName name="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable51" hidden="1">[0]!Table5</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable4" hidden="1">[0]!Table4</definedName>
+    <definedName name="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable5" hidden="1">[0]!Table5</definedName>
     <definedName name="Income_tax_with_children">MAX(0, 'Named formulas'!XFC1*_Taxes2013!$D$6-IF('Named formulas'!XFD1&lt;=2,'Named formulas'!XFD1*_Taxes2013!$I$1,'Named formulas'!XFD1*_Taxes2013!$I$2))</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -50,7 +50,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table4-f70e2b63-73bb-4417-bff9-6eef45bf972c">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable41"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable4"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -59,7 +59,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table5-3d9ae4cd-538f-4ccd-92fa-7604e76ab7a4">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable51"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_TaxCalculation.feature.xlsxTable5"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>Szociális hozzájárulási adó</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>preview:</t>
-  </si>
-  <si>
-    <t>#</t>
   </si>
   <si>
     <t>But</t>
@@ -533,19 +530,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -558,6 +543,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
@@ -569,7 +566,28 @@
       <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
@@ -600,28 +618,7 @@
       <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-* #,##0\ [$Ft-40E]_-;\-* #,##0\ [$Ft-40E]_-;_-* &quot;-&quot;\ [$Ft-40E]_-;_-@_-"/>
@@ -688,9 +685,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="gross" dataDxfId="2"/>
-    <tableColumn id="3" name="children" dataDxfId="1"/>
-    <tableColumn id="2" name="net" dataDxfId="6">
+    <tableColumn id="1" name="gross" dataDxfId="16"/>
+    <tableColumn id="3" name="children" dataDxfId="15"/>
+    <tableColumn id="2" name="net" dataDxfId="14">
       <calculatedColumnFormula>B8-(G8+J8)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -707,16 +704,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Social Security Contributions" dataDxfId="0">
+    <tableColumn id="1" name="Social Security Contributions" dataDxfId="13">
       <calculatedColumnFormula>$B8*SUM(_Taxes2013!$D$3:$D$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Gross" dataDxfId="5">
+    <tableColumn id="4" name="Gross" dataDxfId="12">
       <calculatedColumnFormula>Table1820[[#This Row],[gross]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Children" dataDxfId="4">
+    <tableColumn id="5" name="Children" dataDxfId="11">
       <calculatedColumnFormula>Table1820[[#This Row],[children]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Income tax" dataDxfId="3">
+    <tableColumn id="6" name="Income tax" dataDxfId="10">
       <calculatedColumnFormula>Income_tax_with_children</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -733,16 +730,16 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Munkaerő-piaci járulék" dataDxfId="16">
+    <tableColumn id="1" name="Munkaerő-piaci járulék" dataDxfId="9">
       <calculatedColumnFormula>"&lt;" &amp; INDIRECT("R" &amp; (ROW($H$9) +1+$H$9) &amp; "C" &amp; COLUMN(E$10),FALSE ) &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Egészségbiztosítási járulék" dataDxfId="15">
+    <tableColumn id="2" name="Egészségbiztosítási járulék" dataDxfId="8">
       <calculatedColumnFormula>"&lt;" &amp; INDIRECT("R" &amp; (ROW($H$9) +1+$H$9) &amp; "C" &amp; COLUMN(F$10),FALSE ) &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Nyugdíjjárulék" dataDxfId="14">
+    <tableColumn id="3" name="Nyugdíjjárulék" dataDxfId="7">
       <calculatedColumnFormula>"&lt;" &amp; INDIRECT("R" &amp; (ROW($H$9) +1+$H$9) &amp; "C" &amp; COLUMN(G$10),FALSE ) &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="SZJA" dataDxfId="13">
+    <tableColumn id="4" name="SZJA" dataDxfId="6">
       <calculatedColumnFormula>"&lt;" &amp; INDIRECT("R" &amp; (ROW($H$9) +1+$H$9) &amp; "C" &amp; COLUMN(H$10),FALSE ) &amp; "&gt;"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -763,20 +760,20 @@
   </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" name="Scenario"/>
-    <tableColumn id="2" name="Gross" dataDxfId="12"/>
-    <tableColumn id="3" name="Net" dataDxfId="11">
+    <tableColumn id="2" name="Gross" dataDxfId="5"/>
+    <tableColumn id="3" name="Net" dataDxfId="4">
       <calculatedColumnFormula>C11*(1-_Taxes2013!$D$10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Munkaerő-piaci járulék" dataDxfId="10">
+    <tableColumn id="4" name="Munkaerő-piaci járulék" dataDxfId="3">
       <calculatedColumnFormula>$C11*VLOOKUP(E$10, _Taxes2013!$C:$D, 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Egészségbiztosítási járulék" dataDxfId="9">
+    <tableColumn id="5" name="Egészségbiztosítási járulék" dataDxfId="2">
       <calculatedColumnFormula>$C11*VLOOKUP(F$10, _Taxes2013!$C:$D, 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Nyugdíjjárulék" dataDxfId="8">
+    <tableColumn id="6" name="Nyugdíjjárulék" dataDxfId="1">
       <calculatedColumnFormula>$C11*VLOOKUP(G$10, _Taxes2013!$C:$D, 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="SZJA" dataDxfId="7">
+    <tableColumn id="7" name="SZJA" dataDxfId="0">
       <calculatedColumnFormula>$C11*VLOOKUP(H$10, _Taxes2013!$C:$D, 2, FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1077,7 +1074,7 @@
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1093,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="22"/>
       <c r="J1" s="17"/>
@@ -1138,7 +1135,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="28"/>
       <c r="J6" s="17"/>
@@ -1239,9 +1236,9 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="31"/>
+        <v>33</v>
+      </c>
+      <c r="C1" s="29"/>
       <c r="D1" s="1"/>
       <c r="I1" s="1"/>
     </row>
@@ -1250,9 +1247,9 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="C2" s="29"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="29"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1270,76 +1267,76 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="31"/>
+        <v>35</v>
+      </c>
+      <c r="C4" s="29"/>
       <c r="D4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="31"/>
+      <c r="C5" s="29"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="C6" s="29"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="30"/>
       <c r="G7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="33" t="s">
         <v>43</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>100000</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="29">
         <v>1</v>
       </c>
       <c r="D8" s="1">
         <f>B8-(G8+J8)</f>
         <v>75500</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="32">
         <f>$B8*SUM(_Taxes2013!$D$3:$D$5)</f>
         <v>18500</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="34">
         <f>Table1820[[#This Row],[gross]]</f>
         <v>100000</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="37">
         <f>Table1820[[#This Row],[children]]</f>
         <v>1</v>
       </c>
-      <c r="J8" s="36">
+      <c r="J8" s="32">
         <f>Income_tax_with_children</f>
         <v>6000</v>
       </c>
@@ -1348,26 +1345,26 @@
       <c r="B9" s="1">
         <v>100000</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="29">
         <v>2</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:D11" si="0">B9-(G9+J9)</f>
         <v>81500</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="32">
         <f>$B9*SUM(_Taxes2013!$D$3:$D$5)</f>
         <v>18500</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="34">
         <f>Table1820[[#This Row],[gross]]</f>
         <v>100000</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="37">
         <f>Table1820[[#This Row],[children]]</f>
         <v>2</v>
       </c>
-      <c r="J9" s="36">
+      <c r="J9" s="32">
         <f>Income_tax_with_children</f>
         <v>0</v>
       </c>
@@ -1376,26 +1373,26 @@
       <c r="B10" s="1">
         <v>200000</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>2</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>151000</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="32">
         <f>$B10*SUM(_Taxes2013!$D$3:$D$5)</f>
         <v>37000</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="34">
         <f>Table1820[[#This Row],[gross]]</f>
         <v>200000</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10" s="37">
         <f>Table1820[[#This Row],[children]]</f>
         <v>2</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="32">
         <f>Income_tax_with_children</f>
         <v>12000</v>
       </c>
@@ -1404,26 +1401,26 @@
       <c r="B11" s="1">
         <v>200000</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="29">
         <v>3</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>163000</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="32">
         <f>$B11*SUM(_Taxes2013!$D$3:$D$5)</f>
         <v>37000</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="34">
         <f>Table1820[[#This Row],[gross]]</f>
         <v>200000</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="37">
         <f>Table1820[[#This Row],[children]]</f>
         <v>3</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J11" s="32">
         <f>Income_tax_with_children</f>
         <v>0</v>
       </c>
@@ -1443,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,8 +1545,14 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
+      <c r="D9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="H9">
-        <f>IF(C32=Table2[[#Headers],[Scenario]], 0, MATCH(C32,Table2[Scenario],))</f>
+        <f>IF(E9=Table2[[#Headers],[Scenario]], 0, MATCH(E9,Table2[Scenario],))</f>
         <v>0</v>
       </c>
     </row>
@@ -1681,104 +1684,93 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9">
       <formula1>$B$10:$B$13</formula1>
     </dataValidation>
   </dataValidations>
@@ -1823,7 +1815,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -1857,14 +1849,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="41"/>
       <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
@@ -1930,7 +1922,7 @@
         <v>0.1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1946,10 +1938,10 @@
         <v>23</v>
       </c>
       <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
         <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="13"/>
@@ -1959,8 +1951,8 @@
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
-      <c r="H7" s="39" t="s">
-        <v>45</v>
+      <c r="H7" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="I7" s="1">
         <v>300000</v>

</xml_diff>